<commit_message>
sn: update the pretas forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/2024/sn_lf_pretas_20407_2_fts.xlsx
+++ b/LF/PreTAS/Senegal/2024/sn_lf_pretas_20407_2_fts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Senegal\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F489680C-4D84-47AA-8909-663BE5F342D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816DDA54-17C3-4071-BBC5-09EDA5A34C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -361,12 +361,6 @@
   </si>
   <si>
     <t>3. Sélectionner la commune</t>
-  </si>
-  <si>
-    <t>4. Entrer le nom de l'école</t>
-  </si>
-  <si>
-    <t>5. Entrer le code de l'école</t>
   </si>
   <si>
     <t>6. Combien d'enfant allez vous enregistrer?</t>
@@ -493,15 +487,6 @@
     <t>Insuffisance du volume de sang dû à la pipette</t>
   </si>
   <si>
-    <t>sn_lf_pretas_20407_2_fts</t>
-  </si>
-  <si>
-    <t>(2024 Juillet) 2. Pre-TAS - Formulaire Résultat FTS V4</t>
-  </si>
-  <si>
-    <t>sn_lf_f_2407</t>
-  </si>
-  <si>
     <t>${d_IDType} = "Scanner"</t>
   </si>
   <si>
@@ -518,6 +503,21 @@
   </si>
   <si>
     <t>${d_final_result} = 'Positif'</t>
+  </si>
+  <si>
+    <t>4. Nom du village</t>
+  </si>
+  <si>
+    <t>5. Code du village</t>
+  </si>
+  <si>
+    <t>sn_lf_f_2407_2</t>
+  </si>
+  <si>
+    <t>(2024 Juillet) 2. Pre-TAS - Formulaire Résultat FTS V2</t>
+  </si>
+  <si>
+    <t>sn_lf_pretas_20407_2_fts_v2</t>
   </si>
 </sst>
 </file>
@@ -1111,11 +1111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1180,7 +1180,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="10" customFormat="1" ht="63">
@@ -1268,7 +1268,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="12"/>
@@ -1293,7 +1293,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>27</v>
@@ -1324,7 +1324,7 @@
         <v>100</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J7" s="28" t="s">
         <v>19</v>
@@ -1355,10 +1355,10 @@
         <v>96</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="32"/>
@@ -1421,7 +1421,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="12"/>
@@ -1444,14 +1444,14 @@
         <v>34</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
       <c r="H13" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="12" t="s">
@@ -1469,14 +1469,14 @@
         <v>92</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="13"/>
       <c r="F14" s="16"/>
       <c r="G14" s="15"/>
       <c r="H14" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="12" t="s">
@@ -1494,18 +1494,18 @@
         <v>93</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="13"/>
       <c r="F15" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G15" s="25" t="s">
         <v>94</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="12" t="s">
@@ -1523,7 +1523,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="25"/>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J16" s="23" t="s">
         <v>19</v>
@@ -1549,13 +1549,13 @@
     </row>
     <row r="17" spans="1:13" s="10" customFormat="1">
       <c r="A17" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="12"/>
@@ -1578,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="12"/>
@@ -1605,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>40</v>
@@ -1630,7 +1630,7 @@
         <v>85</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="12"/>
@@ -1655,7 +1655,7 @@
         <v>86</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="12"/>
@@ -1674,13 +1674,13 @@
     </row>
     <row r="22" spans="1:13" s="10" customFormat="1">
       <c r="A22" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="12"/>
@@ -1728,7 +1728,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
@@ -1751,7 +1751,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="12"/>
@@ -1780,7 +1780,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>40</v>
@@ -1807,7 +1807,7 @@
         <v>88</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="11"/>
@@ -1832,7 +1832,7 @@
         <v>89</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="11"/>
@@ -1851,13 +1851,13 @@
     </row>
     <row r="29" spans="1:13" s="10" customFormat="1">
       <c r="A29" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="12"/>
@@ -1888,7 +1888,7 @@
       <c r="G30" s="18"/>
       <c r="H30" s="12"/>
       <c r="I30" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
@@ -1918,20 +1918,20 @@
     </row>
     <row r="32" spans="1:13" s="22" customFormat="1">
       <c r="A32" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
       <c r="H32" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20" t="s">
@@ -1949,7 +1949,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="11"/>
@@ -2141,7 +2141,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>69</v>
@@ -2152,7 +2152,7 @@
         <v>91</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>70</v>
@@ -2163,7 +2163,7 @@
         <v>91</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>71</v>
@@ -2174,7 +2174,7 @@
         <v>91</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>72</v>
@@ -2185,10 +2185,10 @@
         <v>91</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2196,10 +2196,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2226,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2250,10 +2250,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>78</v>

</xml_diff>